<commit_message>
Drobné změny v kódu + dokumentace
</commit_message>
<xml_diff>
--- a/Podklady/Tabulky.xlsx
+++ b/Podklady/Tabulky.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8BDC510-42EF-4FC0-93F7-CF0949F4A45A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3ACAAF-42CE-4683-81F4-C020B6F6162C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Knihovny" sheetId="1" r:id="rId1"/>
-    <sheet name="Parametry Wemos D1" sheetId="3" r:id="rId2"/>
-    <sheet name="Parametry_desky" sheetId="2" r:id="rId3"/>
+    <sheet name="Seznam stránek" sheetId="4" r:id="rId2"/>
+    <sheet name="Parametry Wemos D1" sheetId="3" r:id="rId3"/>
+    <sheet name="Parametry_desky" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="128">
   <si>
     <t>Použité knihovny</t>
   </si>
@@ -238,6 +239,174 @@
   </si>
   <si>
     <t>4MB</t>
+  </si>
+  <si>
+    <t>ESP8266mDNS.h</t>
+  </si>
+  <si>
+    <t>Multicast DNS</t>
+  </si>
+  <si>
+    <t>void handleMain();</t>
+  </si>
+  <si>
+    <t>void handleNotFound();</t>
+  </si>
+  <si>
+    <t>void handleLogin();</t>
+  </si>
+  <si>
+    <t>void handleSetTime();</t>
+  </si>
+  <si>
+    <t>void handleSetMessage();</t>
+  </si>
+  <si>
+    <t>void handleAlarm();</t>
+  </si>
+  <si>
+    <t>void handleAlarmMessage();</t>
+  </si>
+  <si>
+    <t>void handleAlarmOff();</t>
+  </si>
+  <si>
+    <t>void handleChLogin();</t>
+  </si>
+  <si>
+    <t>void handleLogout();</t>
+  </si>
+  <si>
+    <t>void handleChLoginMessage();</t>
+  </si>
+  <si>
+    <t>void handleAccess();</t>
+  </si>
+  <si>
+    <t>void handleAccessMessage();</t>
+  </si>
+  <si>
+    <t>void handleNTP();</t>
+  </si>
+  <si>
+    <t>void handleNTPMessage();</t>
+  </si>
+  <si>
+    <t>void handleRoot();</t>
+  </si>
+  <si>
+    <t>Funkce pro jednotlivé stránky</t>
+  </si>
+  <si>
+    <t>Účel</t>
+  </si>
+  <si>
+    <t>Přihlašovací okno</t>
+  </si>
+  <si>
+    <t>Hlavní obrazovka</t>
+  </si>
+  <si>
+    <t>Chybný parametr</t>
+  </si>
+  <si>
+    <t>Kontrola autorizace</t>
+  </si>
+  <si>
+    <t>Nastavení času</t>
+  </si>
+  <si>
+    <t>Zpracování dat z času</t>
+  </si>
+  <si>
+    <t>Nastavení budíčku</t>
+  </si>
+  <si>
+    <t>Zpracování dat z budíčku</t>
+  </si>
+  <si>
+    <t>Zpracování dat - vypnutí budíčku</t>
+  </si>
+  <si>
+    <t>Změna hesla</t>
+  </si>
+  <si>
+    <t>Metoda</t>
+  </si>
+  <si>
+    <t>Zpracování dat - změna hesla</t>
+  </si>
+  <si>
+    <t>Odhlášení</t>
+  </si>
+  <si>
+    <t>Zpracování dat</t>
+  </si>
+  <si>
+    <t>Nastavení parametrů NTP</t>
+  </si>
+  <si>
+    <t>Zpracování dat z NTP</t>
+  </si>
+  <si>
+    <t>Přípona</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>/main</t>
+  </si>
+  <si>
+    <t>/login</t>
+  </si>
+  <si>
+    <t>/alarm</t>
+  </si>
+  <si>
+    <t>/logout</t>
+  </si>
+  <si>
+    <t>/access</t>
+  </si>
+  <si>
+    <t>/ntp</t>
+  </si>
+  <si>
+    <t>/ntpmessage</t>
+  </si>
+  <si>
+    <t>/settime</t>
+  </si>
+  <si>
+    <t>/setmessage</t>
+  </si>
+  <si>
+    <t>/alarmmessage</t>
+  </si>
+  <si>
+    <t>/alarmoff</t>
+  </si>
+  <si>
+    <t>/chlogin</t>
+  </si>
+  <si>
+    <t>/chloginmessage</t>
+  </si>
+  <si>
+    <t>/accessmessage</t>
+  </si>
+  <si>
+    <t>Změna přihlašovacích údajů k Wi-Fi</t>
   </si>
 </sst>
 </file>
@@ -350,7 +519,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -371,6 +540,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -652,10 +827,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,16 +879,283 @@
         <v>8</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1217BFB-224B-40BF-95F9-F81867AF4CF1}">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C95C3C9-72A9-4FB6-B01C-2250F48E2DA6}">
   <dimension ref="A3:H29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="F13" sqref="F13:H29"/>
     </sheetView>
   </sheetViews>
@@ -998,11 +1440,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7BC677F-C468-41D7-B459-419720B791C6}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A19" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>